<commit_message>
Multiples modificaciones y correcciones
</commit_message>
<xml_diff>
--- a/Archivo_Importacion_Inventario_vehiculos.xlsx
+++ b/Archivo_Importacion_Inventario_vehiculos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="140">
   <si>
     <t>0214445</t>
   </si>
@@ -194,6 +194,246 @@
   </si>
   <si>
     <t>68LTS</t>
+  </si>
+  <si>
+    <t>0214454</t>
+  </si>
+  <si>
+    <t>2ASD10D</t>
+  </si>
+  <si>
+    <t>5S5A14</t>
+  </si>
+  <si>
+    <t>DAD52330</t>
+  </si>
+  <si>
+    <t>69LTS</t>
+  </si>
+  <si>
+    <t>0214455</t>
+  </si>
+  <si>
+    <t>2ASD11D</t>
+  </si>
+  <si>
+    <t>5S5A15</t>
+  </si>
+  <si>
+    <t>DAD52331</t>
+  </si>
+  <si>
+    <t>70LTS</t>
+  </si>
+  <si>
+    <t>0214456</t>
+  </si>
+  <si>
+    <t>2ASD12D</t>
+  </si>
+  <si>
+    <t>5S5A16</t>
+  </si>
+  <si>
+    <t>DAD52332</t>
+  </si>
+  <si>
+    <t>71LTS</t>
+  </si>
+  <si>
+    <t>0214457</t>
+  </si>
+  <si>
+    <t>2ASD13D</t>
+  </si>
+  <si>
+    <t>5S5A17</t>
+  </si>
+  <si>
+    <t>DAD52333</t>
+  </si>
+  <si>
+    <t>72LTS</t>
+  </si>
+  <si>
+    <t>0214458</t>
+  </si>
+  <si>
+    <t>2ASD14D</t>
+  </si>
+  <si>
+    <t>5S5A18</t>
+  </si>
+  <si>
+    <t>DAD52334</t>
+  </si>
+  <si>
+    <t>73LTS</t>
+  </si>
+  <si>
+    <t>0214459</t>
+  </si>
+  <si>
+    <t>2ASD15D</t>
+  </si>
+  <si>
+    <t>5S5A19</t>
+  </si>
+  <si>
+    <t>DAD52335</t>
+  </si>
+  <si>
+    <t>74LTS</t>
+  </si>
+  <si>
+    <t>0214460</t>
+  </si>
+  <si>
+    <t>2ASD16D</t>
+  </si>
+  <si>
+    <t>5S5A20</t>
+  </si>
+  <si>
+    <t>DAD52336</t>
+  </si>
+  <si>
+    <t>75LTS</t>
+  </si>
+  <si>
+    <t>0214461</t>
+  </si>
+  <si>
+    <t>2ASD17D</t>
+  </si>
+  <si>
+    <t>5S5A21</t>
+  </si>
+  <si>
+    <t>DAD52337</t>
+  </si>
+  <si>
+    <t>76LTS</t>
+  </si>
+  <si>
+    <t>0214462</t>
+  </si>
+  <si>
+    <t>2ASD18D</t>
+  </si>
+  <si>
+    <t>5S5A22</t>
+  </si>
+  <si>
+    <t>DAD52338</t>
+  </si>
+  <si>
+    <t>77LTS</t>
+  </si>
+  <si>
+    <t>0214463</t>
+  </si>
+  <si>
+    <t>2ASD19D</t>
+  </si>
+  <si>
+    <t>5S5A23</t>
+  </si>
+  <si>
+    <t>DAD52339</t>
+  </si>
+  <si>
+    <t>78LTS</t>
+  </si>
+  <si>
+    <t>0214464</t>
+  </si>
+  <si>
+    <t>2ASD20D</t>
+  </si>
+  <si>
+    <t>5S5A24</t>
+  </si>
+  <si>
+    <t>DAD52340</t>
+  </si>
+  <si>
+    <t>79LTS</t>
+  </si>
+  <si>
+    <t>0214465</t>
+  </si>
+  <si>
+    <t>2ASD21D</t>
+  </si>
+  <si>
+    <t>5S5A25</t>
+  </si>
+  <si>
+    <t>DAD52341</t>
+  </si>
+  <si>
+    <t>80LTS</t>
+  </si>
+  <si>
+    <t>0214466</t>
+  </si>
+  <si>
+    <t>2ASD22D</t>
+  </si>
+  <si>
+    <t>5S5A26</t>
+  </si>
+  <si>
+    <t>DAD52342</t>
+  </si>
+  <si>
+    <t>81LTS</t>
+  </si>
+  <si>
+    <t>0214467</t>
+  </si>
+  <si>
+    <t>2ASD23D</t>
+  </si>
+  <si>
+    <t>5S5A27</t>
+  </si>
+  <si>
+    <t>DAD52343</t>
+  </si>
+  <si>
+    <t>82LTS</t>
+  </si>
+  <si>
+    <t>0214468</t>
+  </si>
+  <si>
+    <t>2ASD24D</t>
+  </si>
+  <si>
+    <t>5S5A28</t>
+  </si>
+  <si>
+    <t>DAD52344</t>
+  </si>
+  <si>
+    <t>83LTS</t>
+  </si>
+  <si>
+    <t>0214469</t>
+  </si>
+  <si>
+    <t>2ASD25D</t>
+  </si>
+  <si>
+    <t>5S5A29</t>
+  </si>
+  <si>
+    <t>DAD52345</t>
+  </si>
+  <si>
+    <t>84LTS</t>
   </si>
 </sst>
 </file>
@@ -201,10 +441,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -222,31 +462,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,9 +478,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,7 +494,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,7 +510,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,6 +569,22 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -316,44 +593,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,7 +608,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,19 +668,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,7 +722,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,133 +788,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,6 +804,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -571,13 +837,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,36 +891,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -664,148 +904,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1138,10 +1378,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AD9"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1986,6 +2226,1478 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>17</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10">
+        <v>2445531</v>
+      </c>
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10">
+        <v>254423</v>
+      </c>
+      <c r="R10" t="s">
+        <v>10</v>
+      </c>
+      <c r="S10">
+        <v>199531240</v>
+      </c>
+      <c r="T10">
+        <v>2014</v>
+      </c>
+      <c r="U10" t="s">
+        <v>14</v>
+      </c>
+      <c r="V10" t="s">
+        <v>15</v>
+      </c>
+      <c r="W10" t="s">
+        <v>16</v>
+      </c>
+      <c r="X10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>44345</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>44345</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>44345</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>44345</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11">
+        <v>2445532</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11">
+        <v>254424</v>
+      </c>
+      <c r="R11" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11">
+        <v>199531241</v>
+      </c>
+      <c r="T11">
+        <v>2015</v>
+      </c>
+      <c r="U11" t="s">
+        <v>14</v>
+      </c>
+      <c r="V11" t="s">
+        <v>15</v>
+      </c>
+      <c r="W11" t="s">
+        <v>16</v>
+      </c>
+      <c r="X11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>44346</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>44346</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>44346</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>44346</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12">
+        <v>2445533</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12">
+        <v>254425</v>
+      </c>
+      <c r="R12" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12">
+        <v>199531242</v>
+      </c>
+      <c r="T12">
+        <v>2016</v>
+      </c>
+      <c r="U12" t="s">
+        <v>14</v>
+      </c>
+      <c r="V12" t="s">
+        <v>15</v>
+      </c>
+      <c r="W12" t="s">
+        <v>16</v>
+      </c>
+      <c r="X12" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>44347</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>44347</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>44347</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>44347</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13">
+        <v>2445534</v>
+      </c>
+      <c r="P13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>254426</v>
+      </c>
+      <c r="R13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13">
+        <v>199531243</v>
+      </c>
+      <c r="T13">
+        <v>2017</v>
+      </c>
+      <c r="U13" t="s">
+        <v>14</v>
+      </c>
+      <c r="V13" t="s">
+        <v>15</v>
+      </c>
+      <c r="W13" t="s">
+        <v>16</v>
+      </c>
+      <c r="X13" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>44348</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>44348</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>44348</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>44348</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>21</v>
+      </c>
+      <c r="H14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" t="s">
+        <v>10</v>
+      </c>
+      <c r="M14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" t="s">
+        <v>12</v>
+      </c>
+      <c r="O14">
+        <v>2445535</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14">
+        <v>254427</v>
+      </c>
+      <c r="R14" t="s">
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <v>199531244</v>
+      </c>
+      <c r="T14">
+        <v>2018</v>
+      </c>
+      <c r="U14" t="s">
+        <v>14</v>
+      </c>
+      <c r="V14" t="s">
+        <v>15</v>
+      </c>
+      <c r="W14" t="s">
+        <v>16</v>
+      </c>
+      <c r="X14" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y14" s="1">
+        <v>44349</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>44349</v>
+      </c>
+      <c r="AA14" s="1">
+        <v>44349</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC14" s="1">
+        <v>44349</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15">
+        <v>2445536</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15">
+        <v>254428</v>
+      </c>
+      <c r="R15" t="s">
+        <v>10</v>
+      </c>
+      <c r="S15">
+        <v>199531245</v>
+      </c>
+      <c r="T15">
+        <v>2019</v>
+      </c>
+      <c r="U15" t="s">
+        <v>14</v>
+      </c>
+      <c r="V15" t="s">
+        <v>15</v>
+      </c>
+      <c r="W15" t="s">
+        <v>16</v>
+      </c>
+      <c r="X15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y15" s="1">
+        <v>44350</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>44350</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>44350</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC15" s="1">
+        <v>44350</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16">
+        <v>2445537</v>
+      </c>
+      <c r="P16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q16">
+        <v>254429</v>
+      </c>
+      <c r="R16" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16">
+        <v>199531246</v>
+      </c>
+      <c r="T16">
+        <v>2020</v>
+      </c>
+      <c r="U16" t="s">
+        <v>14</v>
+      </c>
+      <c r="V16" t="s">
+        <v>15</v>
+      </c>
+      <c r="W16" t="s">
+        <v>16</v>
+      </c>
+      <c r="X16" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y16" s="1">
+        <v>44351</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>44351</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>44351</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>44351</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
+      <c r="A17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M17" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17">
+        <v>2445538</v>
+      </c>
+      <c r="P17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q17">
+        <v>254430</v>
+      </c>
+      <c r="R17" t="s">
+        <v>10</v>
+      </c>
+      <c r="S17">
+        <v>199531247</v>
+      </c>
+      <c r="T17">
+        <v>2021</v>
+      </c>
+      <c r="U17" t="s">
+        <v>14</v>
+      </c>
+      <c r="V17" t="s">
+        <v>15</v>
+      </c>
+      <c r="W17" t="s">
+        <v>16</v>
+      </c>
+      <c r="X17" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y17" s="1">
+        <v>44352</v>
+      </c>
+      <c r="Z17" s="1">
+        <v>44352</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>44352</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>44352</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
+      <c r="A18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>25</v>
+      </c>
+      <c r="H18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18">
+        <v>2445539</v>
+      </c>
+      <c r="P18" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q18">
+        <v>254431</v>
+      </c>
+      <c r="R18" t="s">
+        <v>10</v>
+      </c>
+      <c r="S18">
+        <v>199531248</v>
+      </c>
+      <c r="T18">
+        <v>2022</v>
+      </c>
+      <c r="U18" t="s">
+        <v>14</v>
+      </c>
+      <c r="V18" t="s">
+        <v>15</v>
+      </c>
+      <c r="W18" t="s">
+        <v>16</v>
+      </c>
+      <c r="X18" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>44353</v>
+      </c>
+      <c r="Z18" s="1">
+        <v>44353</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>44353</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>44353</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
+      <c r="A19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19">
+        <v>2445540</v>
+      </c>
+      <c r="P19" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q19">
+        <v>254432</v>
+      </c>
+      <c r="R19" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19">
+        <v>199531249</v>
+      </c>
+      <c r="T19">
+        <v>2023</v>
+      </c>
+      <c r="U19" t="s">
+        <v>14</v>
+      </c>
+      <c r="V19" t="s">
+        <v>15</v>
+      </c>
+      <c r="W19" t="s">
+        <v>16</v>
+      </c>
+      <c r="X19" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>44354</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>44354</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>44354</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>44354</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="A20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N20" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20">
+        <v>2445541</v>
+      </c>
+      <c r="P20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q20">
+        <v>254433</v>
+      </c>
+      <c r="R20" t="s">
+        <v>10</v>
+      </c>
+      <c r="S20">
+        <v>199531250</v>
+      </c>
+      <c r="T20">
+        <v>2024</v>
+      </c>
+      <c r="U20" t="s">
+        <v>14</v>
+      </c>
+      <c r="V20" t="s">
+        <v>15</v>
+      </c>
+      <c r="W20" t="s">
+        <v>16</v>
+      </c>
+      <c r="X20" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>44355</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>44355</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>44355</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>44355</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
+      <c r="A21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>28</v>
+      </c>
+      <c r="H21" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O21">
+        <v>2445542</v>
+      </c>
+      <c r="P21" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q21">
+        <v>254434</v>
+      </c>
+      <c r="R21" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21">
+        <v>199531251</v>
+      </c>
+      <c r="T21">
+        <v>2025</v>
+      </c>
+      <c r="U21" t="s">
+        <v>14</v>
+      </c>
+      <c r="V21" t="s">
+        <v>15</v>
+      </c>
+      <c r="W21" t="s">
+        <v>16</v>
+      </c>
+      <c r="X21" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y21" s="1">
+        <v>44356</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>44356</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>44356</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>44356</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22">
+        <v>2445543</v>
+      </c>
+      <c r="P22" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q22">
+        <v>254435</v>
+      </c>
+      <c r="R22" t="s">
+        <v>10</v>
+      </c>
+      <c r="S22">
+        <v>199531252</v>
+      </c>
+      <c r="T22">
+        <v>2026</v>
+      </c>
+      <c r="U22" t="s">
+        <v>14</v>
+      </c>
+      <c r="V22" t="s">
+        <v>15</v>
+      </c>
+      <c r="W22" t="s">
+        <v>16</v>
+      </c>
+      <c r="X22" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y22" s="1">
+        <v>44357</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>44357</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>44357</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>44357</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30">
+      <c r="A23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K23" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23">
+        <v>2445544</v>
+      </c>
+      <c r="P23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q23">
+        <v>254436</v>
+      </c>
+      <c r="R23" t="s">
+        <v>10</v>
+      </c>
+      <c r="S23">
+        <v>199531253</v>
+      </c>
+      <c r="T23">
+        <v>2027</v>
+      </c>
+      <c r="U23" t="s">
+        <v>14</v>
+      </c>
+      <c r="V23" t="s">
+        <v>15</v>
+      </c>
+      <c r="W23" t="s">
+        <v>16</v>
+      </c>
+      <c r="X23" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>44358</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>44358</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>44358</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>44358</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30">
+      <c r="A24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
+        <v>131</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <v>31</v>
+      </c>
+      <c r="H24" t="s">
+        <v>132</v>
+      </c>
+      <c r="I24" t="s">
+        <v>133</v>
+      </c>
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+      <c r="K24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24">
+        <v>2445545</v>
+      </c>
+      <c r="P24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q24">
+        <v>254437</v>
+      </c>
+      <c r="R24" t="s">
+        <v>10</v>
+      </c>
+      <c r="S24">
+        <v>199531254</v>
+      </c>
+      <c r="T24">
+        <v>2028</v>
+      </c>
+      <c r="U24" t="s">
+        <v>14</v>
+      </c>
+      <c r="V24" t="s">
+        <v>15</v>
+      </c>
+      <c r="W24" t="s">
+        <v>16</v>
+      </c>
+      <c r="X24" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y24" s="1">
+        <v>44359</v>
+      </c>
+      <c r="Z24" s="1">
+        <v>44359</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>44359</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>44359</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>137</v>
+      </c>
+      <c r="I25" t="s">
+        <v>138</v>
+      </c>
+      <c r="J25" t="s">
+        <v>8</v>
+      </c>
+      <c r="K25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" t="s">
+        <v>11</v>
+      </c>
+      <c r="N25" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25">
+        <v>2445546</v>
+      </c>
+      <c r="P25" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25">
+        <v>254438</v>
+      </c>
+      <c r="R25" t="s">
+        <v>10</v>
+      </c>
+      <c r="S25">
+        <v>199531255</v>
+      </c>
+      <c r="T25">
+        <v>2029</v>
+      </c>
+      <c r="U25" t="s">
+        <v>14</v>
+      </c>
+      <c r="V25" t="s">
+        <v>15</v>
+      </c>
+      <c r="W25" t="s">
+        <v>16</v>
+      </c>
+      <c r="X25" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>44360</v>
+      </c>
+      <c r="Z25" s="1">
+        <v>44360</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>44360</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>44360</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>